<commit_message>
github now public! Readme updated, sections added.
</commit_message>
<xml_diff>
--- a/glottodata.xlsx
+++ b/glottodata.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -418,6 +418,94 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ticu1245</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>orej1242</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>nade1244</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>mara1409</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Glottolog: reset date last modified if glottolog is up-to-date.
</commit_message>
<xml_diff>
--- a/glottodata.xlsx
+++ b/glottodata.xlsx
@@ -7,7 +7,13 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="glottodata" sheetId="1" r:id="rId1"/>
+    <sheet name="structure" sheetId="2" r:id="rId2"/>
+    <sheet name="metadata" sheetId="3" r:id="rId3"/>
+    <sheet name="references" sheetId="4" r:id="rId4"/>
+    <sheet name="remarks" sheetId="5" r:id="rId5"/>
+    <sheet name="readme" sheetId="6" r:id="rId6"/>
+    <sheet name="lookup" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -351,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -385,21 +391,6 @@
           <t>yucu1253</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -407,102 +398,432 @@
           <t>tani1257</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>varname</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>levels</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>groups</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>subgroups</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>var001</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>var002</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ticu1245</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>var003</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>varname</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>reference</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>remarks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>var001</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>var002</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>var003</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>glottocode</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>var001_ref</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>var001_page</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>var002_ref</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>var002_page</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>var003_ref</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>var003_page</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>yucu1253</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>tani1257</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>glottocode</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>var001_remark</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>var002_remark</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>var003_remark</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>yucu1253</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>tani1257</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>info</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>maintainer</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>citation</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>orej1242</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>N</t>
+          <t>url</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>nade1244</t>
+          <t>This database was created using the glottospace R package</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>version 0.0.71</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>type_lookup</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>type_legend</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>symm</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Symmetric binary: positive match is considered the same as a negative match. Variable has three possible values: Y, N, NA where NA stands for missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>asymm</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Asymmetric binary: positive match and negative match are not equal. Variable has three possible values: Y, N, NA where NA stands for missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>factor</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nominal variables. Levels should be given by a letter or abbreviation. For example: A, B, C. NA stands for missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ordered</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ordinal variables. NA stands for missing value</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>numeric</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Interval scaled variables. Can have any numeric value and NA</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>mara1409</t>
+          <t>ordratio</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>N</t>
+          <t>Ratio scaled variables. Setting type to ordratio indicates that values should be treated as ordinal variables</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>logratio</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Ratio scaled variables. Setting type to logratio indicates that values should be log transformed in subsequent analyses</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
glottocreate: add/modify metatables for description, references and contributors. Fixes #49
</commit_message>
<xml_diff>
--- a/glottodata.xlsx
+++ b/glottodata.xlsx
@@ -9,11 +9,12 @@
   <sheets>
     <sheet name="glottodata" sheetId="1" r:id="rId1"/>
     <sheet name="structure" sheetId="2" r:id="rId2"/>
-    <sheet name="metadata" sheetId="3" r:id="rId3"/>
+    <sheet name="description" sheetId="3" r:id="rId3"/>
     <sheet name="references" sheetId="4" r:id="rId4"/>
     <sheet name="remarks" sheetId="5" r:id="rId5"/>
-    <sheet name="readme" sheetId="6" r:id="rId6"/>
-    <sheet name="lookup" sheetId="7" r:id="rId7"/>
+    <sheet name="contributors" sheetId="6" r:id="rId6"/>
+    <sheet name="readme" sheetId="7" r:id="rId7"/>
+    <sheet name="lookup" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -481,7 +482,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -505,17 +506,42 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>page</t>
+          <t>remarks</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>contributor</t>
+          <t>lev_Y</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>remarks</t>
+          <t>lev_N</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>lev_NA</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>lev_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>lev_B</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>lev_C</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>lev_D</t>
         </is>
       </c>
     </row>
@@ -547,7 +573,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -561,30 +587,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>reference</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>var001_ref</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>var001_page</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>var002_ref</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>var002_page</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>var003_ref</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>var003_page</t>
         </is>
@@ -611,7 +647,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -625,15 +661,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>remark</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>var001_remark</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>var002_remark</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>var003_remark</t>
         </is>
@@ -659,6 +700,60 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>glottocode</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>var001_contributor</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>var002_contributor</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>var003_contributor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>yucu1253</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>tani1257</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -723,7 +818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B8"/>
   <sheetViews>

</xml_diff>